<commit_message>
fix: connectionTime and disconnectionTime implemented on charging simulation
</commit_message>
<xml_diff>
--- a/Exports/charging_data.xlsx
+++ b/Exports/charging_data.xlsx
@@ -481,10 +481,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>15.5</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -495,10 +495,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -509,10 +509,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>26.5</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -523,10 +523,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -537,10 +537,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>37.5</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -551,10 +551,10 @@
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -565,10 +565,10 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>48.5</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -579,10 +579,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -593,10 +593,10 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>59.5</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -607,10 +607,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="D12" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -621,10 +621,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>70.5</v>
+        <v>10</v>
       </c>
       <c r="D13" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -635,10 +635,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="D14" t="n">
-        <v>2.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -649,7 +649,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="n">
-        <v>81.5</v>
+        <v>16.875</v>
       </c>
       <c r="D15" t="n">
         <v>2.75</v>
@@ -663,7 +663,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="n">
-        <v>87</v>
+        <v>23.75</v>
       </c>
       <c r="D16" t="n">
         <v>2.75</v>
@@ -677,7 +677,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="n">
-        <v>92.5</v>
+        <v>30.625</v>
       </c>
       <c r="D17" t="n">
         <v>2.75</v>
@@ -691,7 +691,7 @@
         <v>11</v>
       </c>
       <c r="C18" t="n">
-        <v>98</v>
+        <v>37.5</v>
       </c>
       <c r="D18" t="n">
         <v>2.75</v>
@@ -705,7 +705,7 @@
         <v>11</v>
       </c>
       <c r="C19" t="n">
-        <v>103.5</v>
+        <v>44.375</v>
       </c>
       <c r="D19" t="n">
         <v>2.75</v>
@@ -716,13 +716,13 @@
         <v>1.5625</v>
       </c>
       <c r="B20" t="n">
-        <v>-7</v>
+        <v>11</v>
       </c>
       <c r="C20" t="n">
-        <v>100</v>
+        <v>51.25</v>
       </c>
       <c r="D20" t="n">
-        <v>-1.75</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="21">
@@ -730,13 +730,13 @@
         <v>1.572916666666667</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C21" t="n">
-        <v>100</v>
+        <v>58.125</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="22">
@@ -744,13 +744,13 @@
         <v>1.583333333333333</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C22" t="n">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="23">
@@ -758,13 +758,13 @@
         <v>1.59375</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C23" t="n">
-        <v>100</v>
+        <v>71.875</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="24">
@@ -772,13 +772,13 @@
         <v>1.604166666666667</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C24" t="n">
-        <v>100</v>
+        <v>78.75</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="25">
@@ -786,13 +786,13 @@
         <v>1.614583333333333</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C25" t="n">
-        <v>100</v>
+        <v>85.625</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="26">
@@ -800,13 +800,13 @@
         <v>1.625</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C26" t="n">
-        <v>100</v>
+        <v>92.5</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="27">
@@ -814,13 +814,13 @@
         <v>1.635416666666667</v>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C27" t="n">
         <v>100</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">

</xml_diff>